<commit_message>
Removed options.host.colorPalette.color code as per the requirement
</commit_message>
<xml_diff>
--- a/documents/Published/Horizontal Funnel/HorizontalFunnelByMAQSoftwareChecklist.xlsx
+++ b/documents/Published/Horizontal Funnel/HorizontalFunnelByMAQSoftwareChecklist.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\v-dhkon\Desktop\HorizontalFunnel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cutom Visual\PowerBI\documents\Published\HorizontalFunnel\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B099DA1-EA3A-47E4-BA8A-9F60BBD73093}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="1" xr2:uid="{4AB92824-63E9-41E2-A760-A81835BDCF59}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{4AB92824-63E9-41E2-A760-A81835BDCF59}"/>
   </bookViews>
   <sheets>
     <sheet name="Features and test cases" sheetId="1" r:id="rId1"/>
@@ -527,17 +528,17 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -855,8 +856,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFD979CE-A2F4-4A57-BF74-C680FEBF31B0}">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1159,7 +1160,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9445F79-59A8-4539-BCC2-AC7C1C772DD6}">
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
@@ -1346,29 +1347,29 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="9">
+      <c r="A17" s="11">
         <v>16</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C17" s="12" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="9"/>
-      <c r="B18" s="12" t="s">
+      <c r="A18" s="11"/>
+      <c r="B18" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="C18" s="11"/>
+      <c r="C18" s="12"/>
     </row>
     <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="9"/>
-      <c r="B19" s="12" t="s">
+      <c r="A19" s="11"/>
+      <c r="B19" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="C19" s="11"/>
+      <c r="C19" s="12"/>
     </row>
     <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="7">
@@ -1382,41 +1383,41 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="9">
+      <c r="A21" s="11">
         <v>18</v>
       </c>
       <c r="B21" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="C21" s="12" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="9"/>
+      <c r="A22" s="11"/>
       <c r="B22" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="C22" s="11"/>
+      <c r="C22" s="12"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="9"/>
+      <c r="A23" s="11"/>
       <c r="B23" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="C23" s="11"/>
+      <c r="C23" s="12"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="9"/>
+      <c r="A24" s="11"/>
       <c r="B24" s="8"/>
-      <c r="C24" s="11"/>
+      <c r="C24" s="12"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="9"/>
+      <c r="A25" s="11"/>
       <c r="B25" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="C25" s="11"/>
+      <c r="C25" s="12"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="7">

</xml_diff>

<commit_message>
Upgraded API to 2.5.0
</commit_message>
<xml_diff>
--- a/documents/Published/Horizontal Funnel/HorizontalFunnelByMAQSoftwareChecklist.xlsx
+++ b/documents/Published/Horizontal Funnel/HorizontalFunnelByMAQSoftwareChecklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PowerBI-CustomVisuals\documents\Published\Horizontal Funnel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git1\documents\Published\Horizontal Funnel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E7C70E8-F15A-4EF9-9222-0E7B791CDA34}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D61163D2-619C-4F6C-A9ED-4F9669BC5C4E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{4AB92824-63E9-41E2-A760-A81835BDCF59}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4AB92824-63E9-41E2-A760-A81835BDCF59}"/>
   </bookViews>
   <sheets>
     <sheet name="Features and test cases" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="105">
   <si>
     <t>S no</t>
   </si>
@@ -253,9 +253,6 @@
   </si>
   <si>
     <t>The value displayed on the tooltip should be same as actual data i.e. No formatting should be applied to the tooltip data</t>
-  </si>
-  <si>
-    <t>Should display default text "Please select 'Series' and 'Primary Measure' values"</t>
   </si>
   <si>
     <t>Update color of labels</t>
@@ -425,6 +422,23 @@
     <t>1. Bookmarks Pane will be visible on the right side
 2. In the Bookmarks Pane, a new entry is added with saved selection state
 3. On clicking the bookmark, the selection state with filtering is restored and visual is rendered accordingly</t>
+  </si>
+  <si>
+    <t>Drillthrough</t>
+  </si>
+  <si>
+    <t>Created custom menu to drill through from one visual to another.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Generate a chart with some data
+2.Create new report page and in DrillThrough add the fields for drillthrough.
+3. Right click on the chart, select the Drillthrough option from the menu. </t>
+  </si>
+  <si>
+    <t>1. On right click of the chart and selecting the drillthrough option from the context-menu , the report will drillthrough to the newly created report page.</t>
+  </si>
+  <si>
+    <t>Should display default text "Please select both 'Series' and 'Primary Measure' values"</t>
   </si>
 </sst>
 </file>
@@ -511,17 +525,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -536,6 +549,10 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -857,10 +874,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFD979CE-A2F4-4A57-BF74-C680FEBF31B0}">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -903,8 +920,8 @@
       <c r="D2" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>65</v>
+      <c r="E2" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -964,8 +981,8 @@
       <c r="B7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>66</v>
+      <c r="C7" t="s">
+        <v>65</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>51</v>
@@ -1075,7 +1092,7 @@
       <c r="B16" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" t="s">
         <v>61</v>
       </c>
       <c r="D16" s="4" t="s">
@@ -1115,7 +1132,7 @@
       <c r="D18" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="E18" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1137,20 +1154,37 @@
       </c>
     </row>
     <row r="20" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A20" s="5">
+      <c r="A20">
         <v>9</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" t="s">
+        <v>96</v>
+      </c>
+      <c r="C20" t="s">
         <v>97</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="D20" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="E20" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="E20" s="4" t="s">
+    </row>
+    <row r="21" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="10">
+        <v>10</v>
+      </c>
+      <c r="B21" s="10" t="s">
         <v>100</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -1174,274 +1208,274 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="6" t="s">
+    </row>
+    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="6">
+        <v>1</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="7">
-        <v>1</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="6">
+        <v>2</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="7">
-        <v>2</v>
-      </c>
-      <c r="B3" s="8" t="s">
+      <c r="C3" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="6">
+        <v>3</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="7">
-        <v>3</v>
-      </c>
-      <c r="B4" s="8" t="s">
+      <c r="C4" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="6">
+        <v>4</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="7">
-        <v>4</v>
-      </c>
-      <c r="B5" s="8" t="s">
+      <c r="C5" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="7">
-        <v>5</v>
-      </c>
-      <c r="B6" s="8" t="s">
+      <c r="C6" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="6">
+        <v>6</v>
+      </c>
+      <c r="B7" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="C6" s="8" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="7">
-        <v>6</v>
-      </c>
-      <c r="B7" s="8" t="s">
+      <c r="C7" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="6">
+        <v>7</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="C7" s="8" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="7">
-        <v>7</v>
-      </c>
-      <c r="B8" s="8" t="s">
+      <c r="C8" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="6">
+        <v>8</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="6">
+        <v>9</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="6">
+        <v>10</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="6">
+        <v>11</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="6">
+        <v>12</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="6">
+        <v>13</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="6">
+        <v>14</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="6">
+        <v>15</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="12">
+        <v>16</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="12"/>
+      <c r="B18" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C18" s="13"/>
+    </row>
+    <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="12"/>
+      <c r="B19" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="C19" s="13"/>
+    </row>
+    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="6">
+        <v>17</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="12">
+        <v>18</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="12"/>
+      <c r="B22" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C22" s="13"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="12"/>
+      <c r="B23" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C23" s="13"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="12"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="13"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="12"/>
+      <c r="B25" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C25" s="13"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="6">
+        <v>19</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="6">
+        <v>20</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C27" s="7" t="s">
         <v>77</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="7">
-        <v>8</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="7">
-        <v>9</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="7">
-        <v>10</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="7">
-        <v>11</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="7">
-        <v>12</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="7">
-        <v>13</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="7">
-        <v>14</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="7">
-        <v>15</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="11">
-        <v>16</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="C17" s="12" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="11"/>
-      <c r="B18" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="C18" s="12"/>
-    </row>
-    <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="11"/>
-      <c r="B19" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="C19" s="12"/>
-    </row>
-    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="7">
-        <v>17</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="11">
-        <v>18</v>
-      </c>
-      <c r="B21" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="C21" s="12" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="11"/>
-      <c r="B22" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="C22" s="12"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="11"/>
-      <c r="B23" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="C23" s="12"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="11"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="12"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="11"/>
-      <c r="B25" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="C25" s="12"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="7">
-        <v>19</v>
-      </c>
-      <c r="B26" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C26" s="8" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="7">
-        <v>20</v>
-      </c>
-      <c r="B27" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="C27" s="8" t="s">
-        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>